<commit_message>
added the instruction in the templates
</commit_message>
<xml_diff>
--- a/Frontend/public/templates/higher_studies_template.xlsx
+++ b/Frontend/public/templates/higher_studies_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\UGSF\UGSF_TNP\Frontend\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="140">
   <si>
     <t>email</t>
   </si>
@@ -94,38 +94,707 @@
     <t>Admitted</t>
   </si>
   <si>
+    <t>University of Oxford</t>
+  </si>
+  <si>
+    <t>University Offices,Wellington Square,Oxford,OX1 2JD,United Kingdom</t>
+  </si>
+  <si>
+    <t>Economics and Management</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Instructions for Filling the Excel Spreadsheet</t>
+  </si>
+  <si>
+    <t>To ensure the data is entered correctly and can be easily analyzed, please follow these guidelines when filling out the Excel spreadsheet:</t>
+  </si>
+  <si>
+    <t>General Guidelines</t>
+  </si>
+  <si>
+    <t>Sheet Structure</t>
+  </si>
+  <si>
+    <t>The Excel file may contain two sheets based on career choice:</t>
+  </si>
+  <si>
+    <t>Alternatively, use a single sheet and differentiate records using the career_choice column.</t>
+  </si>
+  <si>
+    <t>Column-Specific Instructions</t>
+  </si>
+  <si>
+    <t>Below are the fields from your templates and how to fill them:</t>
+  </si>
+  <si>
+    <t>Common Fields (Applicable to Both Sheets)</t>
+  </si>
+  <si>
+    <t>Use sentence case (capitalize first letters of each word).</t>
+  </si>
+  <si>
+    <t>Ensure it follows standard email format (username@domain.com).</t>
+  </si>
+  <si>
+    <t>Enter the unique enrollment ID (e.g., "22DCE001").</t>
+  </si>
+  <si>
+    <t>Format: Typically a combination of year and program code followed by a number.</t>
+  </si>
+  <si>
+    <t>Enter the year of enrollment as a 4-digit number (e.g., "2022").</t>
+  </si>
+  <si>
+    <t>Enter the batch year (e.g., "2022").</t>
+  </si>
+  <si>
+    <t>Specify either "Higher Studies" or "Job Placement".</t>
+  </si>
+  <si>
+    <t>This determines which additional fields apply.</t>
+  </si>
+  <si>
+    <t>Enter the current semester (e.g., "SEM 8").</t>
+  </si>
+  <si>
+    <t>Use "SEM" followed by a space and the semester number.</t>
+  </si>
+  <si>
+    <t>Enter the full name of the university (e.g., "University of Oxford").</t>
+  </si>
+  <si>
+    <t>Specify the course or degree program (e.g., "Economics and Management").</t>
+  </si>
+  <si>
+    <t>Enter the area of focus, if applicable (e.g., "Leadership"). Use "N/A" if none.</t>
+  </si>
+  <si>
+    <t>Enter the year of admission to the higher studies program (e.g., "2026").</t>
+  </si>
+  <si>
+    <t>Provide the full address, including postal code (e.g., "University Offices, Wellington Square, Oxford, OX1 2JD, United Kingdom").</t>
+  </si>
+  <si>
+    <t>Enter the city where the institute is located (e.g., "Oxford").</t>
+  </si>
+  <si>
+    <t>Enter the country (e.g., "England").</t>
+  </si>
+  <si>
+    <t>Indicate status: "Admitted", "Applied", or "Pending".</t>
+  </si>
+  <si>
+    <t>Job Placement Sheet (For career_choice = "Job Placement")</t>
+  </si>
+  <si>
+    <t>Enter the name of the company (e.g., "Apple").</t>
+  </si>
+  <si>
+    <t>Enter the salary package as a numeric value (e.g., "2500000").</t>
+  </si>
+  <si>
+    <t>Use the local currency (assumed INR unless specified).</t>
+  </si>
+  <si>
+    <t>Indicate status: "Placed", "Offer Received", or "In Progress".</t>
+  </si>
+  <si>
+    <t>Example Data Entry</t>
+  </si>
+  <si>
+    <t>enrollment_year: 2022</t>
+  </si>
+  <si>
+    <t>batch: 2022</t>
+  </si>
+  <si>
+    <t>program: DCE</t>
+  </si>
+  <si>
+    <t>career_choice: Higher Studies</t>
+  </si>
+  <si>
+    <t>semester: SEM 8</t>
+  </si>
+  <si>
+    <t>university_name: University of Oxford</t>
+  </si>
+  <si>
+    <t>course_name: Economics and Management</t>
+  </si>
+  <si>
+    <t>specialization: Leadership</t>
+  </si>
+  <si>
+    <t>admission_year: 2026</t>
+  </si>
+  <si>
+    <t>address_of_institute: University Offices, Wellington Square, Oxford, OX1 2JD, United Kingdom</t>
+  </si>
+  <si>
+    <t>city_of_institute: Oxford</t>
+  </si>
+  <si>
+    <t>country_of_institute: England</t>
+  </si>
+  <si>
+    <t>higher_studies_status: Admitted</t>
+  </si>
+  <si>
+    <t>career_choice: Job Placement</t>
+  </si>
+  <si>
+    <t>company_name: Apple</t>
+  </si>
+  <si>
+    <t>position: SDE</t>
+  </si>
+  <si>
+    <t>package: 2500000</t>
+  </si>
+  <si>
+    <t>placement_status: Placed</t>
+  </si>
+  <si>
+    <t>Enter the full name of the student (e.g., "Paghdar Vedant").</t>
+  </si>
+  <si>
+    <t>Enter a valid email address (e.g., "22dce059@charusat.edu.in" or "name@gmail.com").</t>
+  </si>
+  <si>
+    <t>Usually matches the enrollment_year unless specified otherwise(eg: D2D students).</t>
+  </si>
+  <si>
+    <t>Enter the program code or name (e.g., "DCE" ,"DCS" , "DIT"). As(DCE represents Depstar CE).</t>
+  </si>
+  <si>
+    <t>Higher Studies Data (For career_choice = "Higher Studies")</t>
+  </si>
+  <si>
+    <t>Specify the job role (e.g., "SDE" for Software Development Engineer or can also enter "Software Development Engineer").</t>
+  </si>
+  <si>
+    <t>name: Paghdar Vedant</t>
+  </si>
+  <si>
+    <t>email: 22DCE059@charusat.edu.in</t>
+  </si>
+  <si>
+    <t>enrollment_id: 22DCE059</t>
+  </si>
+  <si>
     <t>Paghdar Vedant</t>
   </si>
   <si>
-    <t>22dce059@charusat.edu.in</t>
+    <t>22DCE059@charusat.edu.in</t>
   </si>
   <si>
     <t>22DCE059</t>
   </si>
   <si>
-    <t>University of Oxford</t>
-  </si>
-  <si>
-    <t>University Offices,Wellington Square,Oxford,OX1 2JD,United Kingdom</t>
-  </si>
-  <si>
-    <t>Economics and Management</t>
-  </si>
-  <si>
-    <t>Leadership</t>
-  </si>
-  <si>
-    <t>Oxford</t>
-  </si>
-  <si>
-    <t>England</t>
+    <r>
+      <t>Sheet 1: Instructions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ( for reference that how to fill the data).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sheet 2: Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ( in this sheet all the data will go).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. enrollment_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4. enrollment_year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5. batch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6. program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7. career_choice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8. semester</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9. university_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10. course_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11. specialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12. admission_year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>13. address_of_institute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>14. city_of_institute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>15. country_of_institute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>16. higher_studies_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9. company_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10. position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11. package</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12. placement_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Higher Studies Row</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Job Placement Row</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Single Sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: All data (Higher Studies and Job Placement) must be entered in one Excel sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. Consistency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Use consistent formatting (e.g., dates as YYYY, text in sentence case unless specified otherwise).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. No Empty Required Cells</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Fill all required fields. If data is unavailable, enter "N/A" or "Pending" as applicable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4. Unique Entries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Each row should represent a unique individual identified by their enrollment_id.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5. Avoid Duplicates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Check that no two rows have the same enrollment_id unless updating an existing record (e.g., career choice change).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6. Accuracy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Double-check spellings, especially for names, email addresses, and institute/company details.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7. Empty Columns Rule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>If career_choice is "Higher Studies", leave all Job Placement-specific columns (company_name, position, package, placement_status) empty or enter "N/A".</t>
+  </si>
+  <si>
+    <t>If career_choice is "Job Placement", leave all Higher Studies-specific columns (university_name, course_name, specialization, admission_year, address_of_institute, city_of_institute, country_of_institute, higher_studies_status) empty or enter "N/A".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     university_name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     course_name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     specialization:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     admission_year:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     address_of_institute:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     city_of_institute:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     country_of_institute:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     higher_studies_status:</t>
+  </si>
+  <si>
+    <t>Just have to empty the higher studies fields as above example</t>
+  </si>
+  <si>
+    <t>company_name:</t>
+  </si>
+  <si>
+    <t>position:</t>
+  </si>
+  <si>
+    <t>package:</t>
+  </si>
+  <si>
+    <t>placement_status:</t>
+  </si>
+  <si>
+    <t>Just have to empty the placements fields as above example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,15 +831,31 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -217,7 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -232,13 +917,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -246,6 +928,43 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,12 +1271,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A135"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="116.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="17"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="17"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="20"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="20"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A35" r:id="rId1" display="mailto:hogrider@gmail.com"/>
+    <hyperlink ref="A36" r:id="rId2" display="mailto:username@domain.com"/>
+    <hyperlink ref="A90" r:id="rId3" display="mailto:hogrider@gmail.com"/>
+    <hyperlink ref="A115" r:id="rId4" display="mailto:hogrider@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -567,7 +1893,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,47 +1919,47 @@
     <col min="20" max="20" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -651,61 +1977,61 @@
       <c r="S1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2022</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7">
-        <v>2022</v>
-      </c>
-      <c r="E2" s="7">
-        <v>2022</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="P2" s="5">
         <v>2026</v>
       </c>
       <c r="Q2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="S2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>